<commit_message>
doct derecho kant 2
</commit_message>
<xml_diff>
--- a/assets uarm/2024 1/larecsm.xlsx
+++ b/assets uarm/2024 1/larecsm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="7395" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="7395"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,6 +789,9 @@
       <c r="C5">
         <v>17</v>
       </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -797,6 +800,9 @@
       <c r="C6">
         <v>17</v>
       </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -813,6 +819,9 @@
       <c r="C8">
         <v>17</v>
       </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -834,6 +843,9 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -850,6 +862,9 @@
       <c r="C13">
         <v>18</v>
       </c>
+      <c r="D13">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -875,15 +890,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -897,7 +915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
avances de algo que no existe
</commit_message>
<xml_diff>
--- a/assets uarm/2024 1/larecsm.xlsx
+++ b/assets uarm/2024 1/larecsm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="7395" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="7395"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +733,18 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -744,6 +756,12 @@
       <c r="D5">
         <v>16</v>
       </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -755,6 +773,12 @@
       <c r="D6">
         <v>17</v>
       </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -763,6 +787,12 @@
       <c r="C7">
         <v>18</v>
       </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -774,6 +804,12 @@
       <c r="D8">
         <v>18</v>
       </c>
+      <c r="E8">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -782,6 +818,15 @@
       <c r="C9">
         <v>18</v>
       </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -790,6 +835,15 @@
       <c r="C10">
         <v>18</v>
       </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -798,6 +852,15 @@
       <c r="C11">
         <v>16</v>
       </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -809,6 +872,12 @@
       <c r="D12">
         <v>17</v>
       </c>
+      <c r="E12">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -820,6 +889,12 @@
       <c r="D13">
         <v>18</v>
       </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -831,6 +906,12 @@
       <c r="D14">
         <v>17</v>
       </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -842,6 +923,12 @@
       <c r="D15">
         <v>16</v>
       </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -853,8 +940,14 @@
       <c r="D16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -864,8 +957,14 @@
       <c r="D17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -879,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,6 +1017,9 @@
       <c r="D4">
         <v>19</v>
       </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -929,6 +1031,9 @@
       <c r="D5">
         <v>20</v>
       </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -940,6 +1045,9 @@
       <c r="D6">
         <v>19</v>
       </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -951,6 +1059,9 @@
       <c r="D7">
         <v>19</v>
       </c>
+      <c r="E7">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -962,6 +1073,9 @@
       <c r="D8">
         <v>20</v>
       </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -973,6 +1087,9 @@
       <c r="D9">
         <v>20</v>
       </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -984,6 +1101,9 @@
       <c r="D10">
         <v>17</v>
       </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -995,6 +1115,9 @@
       <c r="D11">
         <v>20</v>
       </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1006,6 +1129,9 @@
       <c r="D12">
         <v>18</v>
       </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -1017,6 +1143,9 @@
       <c r="D13">
         <v>20</v>
       </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -1028,6 +1157,9 @@
       <c r="D14">
         <v>20</v>
       </c>
+      <c r="E14">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -1039,6 +1171,9 @@
       <c r="D15">
         <v>20</v>
       </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -1050,8 +1185,11 @@
       <c r="D16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
@@ -1061,8 +1199,11 @@
       <c r="D17">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1072,8 +1213,11 @@
       <c r="D18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1083,8 +1227,11 @@
       <c r="D19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
@@ -1094,8 +1241,11 @@
       <c r="D20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>112</v>
       </c>
@@ -1105,8 +1255,11 @@
       <c r="D21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1116,8 +1269,11 @@
       <c r="D22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1127,8 +1283,11 @@
       <c r="D23">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1138,8 +1297,11 @@
       <c r="D24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1149,8 +1311,11 @@
       <c r="D25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1160,8 +1325,11 @@
       <c r="D26">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>46</v>
       </c>
@@ -1171,8 +1339,11 @@
       <c r="D27">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1182,8 +1353,11 @@
       <c r="D28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1193,8 +1367,11 @@
       <c r="D29">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
@@ -1204,8 +1381,11 @@
       <c r="D30">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
@@ -1216,7 +1396,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>51</v>
       </c>
@@ -1226,8 +1406,11 @@
       <c r="D32">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
@@ -1237,8 +1420,11 @@
       <c r="D33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>53</v>
       </c>
@@ -1246,15 +1432,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>55</v>
       </c>
@@ -1264,8 +1453,11 @@
       <c r="D36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>56</v>
       </c>
@@ -1274,6 +1466,9 @@
       </c>
       <c r="D37">
         <v>19</v>
+      </c>
+      <c r="E37">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1286,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,6 +1520,9 @@
       <c r="D4">
         <v>15</v>
       </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1336,6 +1534,9 @@
       <c r="D5">
         <v>16</v>
       </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -1347,6 +1548,9 @@
       <c r="D6">
         <v>10</v>
       </c>
+      <c r="E6">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1358,6 +1562,9 @@
       <c r="D7">
         <v>16</v>
       </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1369,6 +1576,9 @@
       <c r="D8">
         <v>20</v>
       </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -1380,6 +1590,9 @@
       <c r="D9">
         <v>20</v>
       </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1391,6 +1604,9 @@
       <c r="D10">
         <v>18</v>
       </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1402,6 +1618,9 @@
       <c r="D11">
         <v>18</v>
       </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1413,6 +1632,9 @@
       <c r="D12">
         <v>17</v>
       </c>
+      <c r="E12">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1424,6 +1646,9 @@
       <c r="D13">
         <v>16</v>
       </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1435,6 +1660,9 @@
       <c r="D14">
         <v>18</v>
       </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1446,6 +1674,9 @@
       <c r="D15">
         <v>20</v>
       </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1454,6 +1685,9 @@
       <c r="C16">
         <v>15</v>
       </c>
+      <c r="E16">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -1465,6 +1699,9 @@
       <c r="D17">
         <v>20</v>
       </c>
+      <c r="E17">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -1476,6 +1713,9 @@
       <c r="D18">
         <v>20</v>
       </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1487,6 +1727,9 @@
       <c r="D19">
         <v>14</v>
       </c>
+      <c r="E19">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -1498,6 +1741,9 @@
       <c r="D20">
         <v>18</v>
       </c>
+      <c r="E20">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -1509,6 +1755,9 @@
       <c r="D21">
         <v>18</v>
       </c>
+      <c r="E21">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -1520,6 +1769,9 @@
       <c r="D22">
         <v>16</v>
       </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -1531,6 +1783,9 @@
       <c r="D23">
         <v>20</v>
       </c>
+      <c r="E23">
+        <v>19</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -1542,6 +1797,9 @@
       <c r="D24">
         <v>18</v>
       </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -1553,6 +1811,9 @@
       <c r="D25">
         <v>14</v>
       </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -1562,7 +1823,10 @@
         <v>15</v>
       </c>
       <c r="D26">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -1575,11 +1839,17 @@
       <c r="D27">
         <v>12</v>
       </c>
+      <c r="E27">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>102</v>
       </c>
+      <c r="E28">
+        <v>19</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -1591,6 +1861,9 @@
       <c r="D29">
         <v>16</v>
       </c>
+      <c r="E29">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -1602,6 +1875,9 @@
       <c r="D30">
         <v>18</v>
       </c>
+      <c r="E30">
+        <v>19</v>
+      </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -1613,6 +1889,9 @@
       <c r="D31">
         <v>18</v>
       </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
       <c r="F31" t="s">
         <v>114</v>
       </c>
@@ -1627,8 +1906,11 @@
       <c r="D32">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>107</v>
       </c>
@@ -1638,8 +1920,11 @@
       <c r="D33">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>108</v>
       </c>
@@ -1649,8 +1934,11 @@
       <c r="D34">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>109</v>
       </c>
@@ -1660,8 +1948,11 @@
       <c r="D35">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>110</v>
       </c>
@@ -1671,8 +1962,11 @@
       <c r="D36">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>111</v>
       </c>
@@ -1681,6 +1975,9 @@
       </c>
       <c r="D37">
         <v>18</v>
+      </c>
+      <c r="E37">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1692,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,6 +2028,9 @@
       <c r="D4">
         <v>17</v>
       </c>
+      <c r="E4">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1747,6 +2047,9 @@
       <c r="D6">
         <v>15</v>
       </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1758,6 +2061,9 @@
       <c r="D7">
         <v>16</v>
       </c>
+      <c r="E7">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1780,6 +2086,9 @@
       <c r="D9">
         <v>14</v>
       </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1791,6 +2100,9 @@
       <c r="D10">
         <v>19</v>
       </c>
+      <c r="E10">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1802,6 +2114,9 @@
       <c r="D11">
         <v>18</v>
       </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1813,6 +2128,9 @@
       <c r="D12">
         <v>17</v>
       </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1824,6 +2142,9 @@
       <c r="D13">
         <v>13</v>
       </c>
+      <c r="E13">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1832,6 +2153,9 @@
       <c r="D14">
         <v>19</v>
       </c>
+      <c r="E14">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1843,6 +2167,9 @@
       <c r="D15">
         <v>20</v>
       </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1854,8 +2181,11 @@
       <c r="D16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>69</v>
       </c>
@@ -1865,8 +2195,11 @@
       <c r="D17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>70</v>
       </c>
@@ -1876,8 +2209,11 @@
       <c r="D18">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>71</v>
       </c>
@@ -1887,8 +2223,11 @@
       <c r="D19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>72</v>
       </c>
@@ -1898,8 +2237,11 @@
       <c r="D20">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>73</v>
       </c>
@@ -1909,8 +2251,11 @@
       <c r="D21">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>74</v>
       </c>
@@ -1920,8 +2265,11 @@
       <c r="D22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>75</v>
       </c>
@@ -1931,8 +2279,11 @@
       <c r="D23">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>76</v>
       </c>
@@ -1942,8 +2293,11 @@
       <c r="D24">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>77</v>
       </c>
@@ -1953,8 +2307,11 @@
       <c r="D25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>78</v>
       </c>
@@ -1963,6 +2320,9 @@
       </c>
       <c r="D26">
         <v>19</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>